<commit_message>
Create new branch - Sept 2021 Connectathon
</commit_message>
<xml_diff>
--- a/IJE Data Elements Mapping.xlsx
+++ b/IJE Data Elements Mapping.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulMalikShakir\Documents\NCHS-20210126T065408Z-001\NCHS\VR_FHIR\VRDR_R4_Publication\September 2021 Connectathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulMalikShakir\Documents\NCHS-20210126T065408Z-001\NCHS\VR_FHIR\VRDR_R4_Publication\vrdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97263D2-04A3-4F12-9533-F6AE848B9AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7B8415-A94C-4BB7-8DE5-A50493A4BF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IJE Data Elements Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IJE Data Elements Mapping'!$A$1:$Z$1000</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -2366,10 +2369,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -34792,6 +34795,7 @@
       <c r="Z1000" s="11"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z1000" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
update dependencies in the PHINVAD branch
</commit_message>
<xml_diff>
--- a/IJE Data Elements Mapping.xlsx
+++ b/IJE Data Elements Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulMalikShakir\Documents\NCHS-20210126T065408Z-001\NCHS\VR_FHIR\VRDR_R4_Publication\vrdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC76C02-CD27-4442-9EAD-5622AF6F6551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11250808-04EF-424C-B512-E8E0D6C769BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2373,14 +2373,14 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
+      <selection pane="bottomRight" activeCell="E72" sqref="E71:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="72.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>

</xml_diff>